<commit_message>
Implemented update and insert functionalities
</commit_message>
<xml_diff>
--- a/FOMS/data/menu_list.xlsx
+++ b/FOMS/data/menu_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71DA07A-6848-4D21-9B8A-5F3FAC4860CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EC2654-2382-4466-AB72-345F74BD2EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="staff" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$A$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$2:$A$88</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -29,90 +29,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>477c0c7e-9d46-4202-969d-f3dd1933a575</t>
+  </si>
+  <si>
+    <t>FRIES</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
   <si>
     <t>NTU</t>
   </si>
   <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>67136f7c-fcd0-45f1-8859-9e3d183faeb3</t>
+  </si>
+  <si>
+    <t>3PC set meal</t>
+  </si>
+  <si>
+    <t>9.9</t>
+  </si>
+  <si>
+    <t>set meal</t>
+  </si>
+  <si>
+    <t>Value meal</t>
+  </si>
+  <si>
+    <t>5cc0e578-41b6-4e7d-b6e8-5f287be3e857</t>
+  </si>
+  <si>
+    <t>Coke</t>
+  </si>
+  <si>
+    <t>JE</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>6cd0a2b8-2412-4c2a-bf28-b52d043d414b</t>
+  </si>
+  <si>
+    <t>COLE SLAW</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>9234b60f-23e1-4b28-9732-c987de0605a8</t>
+  </si>
+  <si>
+    <t>22148748-4c7e-4331-8686-d2c6d3c27e22</t>
+  </si>
+  <si>
+    <t>chicken nugget</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
-    <t>JE</t>
-  </si>
-  <si>
-    <t>chicken nugget</t>
-  </si>
-  <si>
-    <t>3PC set meal</t>
-  </si>
-  <si>
-    <t>CAJUN FISH</t>
-  </si>
-  <si>
-    <t>FRIES</t>
-  </si>
-  <si>
-    <t>COLE SLAW</t>
-  </si>
-  <si>
-    <t>side</t>
-  </si>
-  <si>
-    <t>burger</t>
-  </si>
-  <si>
-    <t>set meal</t>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>ec084e54-155c-4a11-b8e8-04df6cfe3c87</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>Nice chicken</t>
+  </si>
+  <si>
+    <t>61606264-3573-4492-abed-5a026cdfc717</t>
   </si>
   <si>
     <t>pepsi</t>
   </si>
   <si>
-    <t>drink</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>branch</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Hot piping fries</t>
-  </si>
-  <si>
-    <t>Value meal</t>
-  </si>
-  <si>
-    <t>Hot piping fish</t>
-  </si>
-  <si>
-    <t>Fresh colesaw</t>
-  </si>
-  <si>
-    <t>Made with the finest chicken</t>
-  </si>
-  <si>
-    <t>Drink</t>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>50% off</t>
   </si>
 </sst>
 </file>
@@ -490,12 +523,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,200 +541,193 @@
     <col min="6" max="16384" width="8.7265625" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>3.2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>9.9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>5.6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>2.7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>10.4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>6.9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>6.6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>2.1</v>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Implemented delete function for serialisation
</commit_message>
<xml_diff>
--- a/FOMS/data/menu_list.xlsx
+++ b/FOMS/data/menu_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -146,12 +146,31 @@
   </si>
   <si>
     <t>50% off</t>
+  </si>
+  <si>
+    <t>6afbf012-02ae-470f-8396-ff1a43790bc2</t>
+  </si>
+  <si>
+    <t>Tomato Soup</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>soup</t>
+  </si>
+  <si>
+    <t>Fresh tomatoes</t>
+  </si>
+  <si>
+    <t>4.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -533,12 +552,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7265625" collapsed="1"/>
-    <col min="5" max="5" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="8.7265625" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.81640625" collapsed="true"/>
+    <col min="4" max="4" width="8.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="6" max="16384" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -701,25 +720,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
@@ -727,7 +729,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
@@ -752,10 +754,10 @@
       <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
@@ -785,10 +787,10 @@
       <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3"/>
+      <c r="A36" s="1"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
@@ -863,10 +865,10 @@
       <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
+      <c r="A61" s="4"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="4"/>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
@@ -906,9 +908,6 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Fixed errors with duplicate entries and menu related tasks
</commit_message>
<xml_diff>
--- a/FOMS/data/menu_list.xlsx
+++ b/FOMS/data/menu_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -173,6 +173,75 @@
   </si>
   <si>
     <t>61455e04-c834-4dd5-b64b-79514dc8ac62</t>
+  </si>
+  <si>
+    <t>0595eb38-9a4f-4a4e-ab06-67019a6f2fa5</t>
+  </si>
+  <si>
+    <t>Fries</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>tasty! yay</t>
+  </si>
+  <si>
+    <t>99105856-cc49-45df-b605-d5989d515319</t>
+  </si>
+  <si>
+    <t>Test tasty</t>
+  </si>
+  <si>
+    <t>9fdbdc80-b998-444e-a3af-0017900c9fc2</t>
+  </si>
+  <si>
+    <t>fries</t>
+  </si>
+  <si>
+    <t>Hot piping fries</t>
+  </si>
+  <si>
+    <t>931fe060-d1b5-487f-9bc4-ab60bd3fa135</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>e71db75f-edef-4691-88aa-f7c7114a725b</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>burger</t>
+  </si>
+  <si>
+    <t>Beef burger</t>
+  </si>
+  <si>
+    <t>7.9</t>
+  </si>
+  <si>
+    <t>Beef burger great deal</t>
+  </si>
+  <si>
+    <t>7f5f1d41-584e-481c-bacd-b8f303e75a6d</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>Test Test</t>
+  </si>
+  <si>
+    <t>52805239-f4e6-494e-935e-59fd932fbb89</t>
+  </si>
+  <si>
+    <t>Chicken tenders</t>
   </si>
 </sst>
 </file>
@@ -551,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -589,44 +658,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -749,16 +818,39 @@
         <v>45</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
@@ -777,13 +869,13 @@
       <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
@@ -810,13 +902,13 @@
       <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
@@ -888,13 +980,13 @@
       <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
+      <c r="A58" s="4"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
+      <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
@@ -931,12 +1023,6 @@
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Enabled proper case functionality
</commit_message>
<xml_diff>
--- a/FOMS/data/menu_list.xlsx
+++ b/FOMS/data/menu_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>name</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>486fa33a-7628-4421-babb-8c3527b50c79</t>
+  </si>
+  <si>
+    <t>ed718b0b-88f1-44cb-b4db-493fcf3ff473</t>
+  </si>
+  <si>
+    <t>Cool Drink</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Half Price!</t>
   </si>
 </sst>
 </file>
@@ -870,8 +882,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
Fixed null pointer error
</commit_message>
<xml_diff>
--- a/FOMS/data/menu_list.xlsx
+++ b/FOMS/data/menu_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -278,6 +278,18 @@
   </si>
   <si>
     <t>Value Meal!</t>
+  </si>
+  <si>
+    <t>33122faf-da93-48ae-a714-6bb7c53ebd81</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>3.3</t>
   </si>
 </sst>
 </file>
@@ -656,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -950,10 +962,10 @@
       <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
@@ -983,10 +995,10 @@
       <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
@@ -1061,10 +1073,10 @@
       <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="1"/>
+      <c r="A56" s="4"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="4"/>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
@@ -1104,9 +1116,6 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>